<commit_message>
régi adatok voltak az excelben, ezt javítottam
</commit_message>
<xml_diff>
--- a/resources/terkep_adatok.xlsx
+++ b/resources/terkep_adatok.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="247">
   <si>
     <t>Koordináta</t>
   </si>
@@ -742,6 +742,24 @@
   </si>
   <si>
     <t>Q9</t>
+  </si>
+  <si>
+    <t>Fegyver típus</t>
+  </si>
+  <si>
+    <t>Maula Pistol</t>
+  </si>
+  <si>
+    <t>Crysknife</t>
+  </si>
+  <si>
+    <t>Lasgun</t>
+  </si>
+  <si>
+    <t>koordináta</t>
+  </si>
+  <si>
+    <t>lc</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K218"/>
+  <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="N204" sqref="N204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,7 +1096,7 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1112,8 +1130,14 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1143,8 +1167,14 @@
       <c r="K2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1174,8 +1204,14 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1209,8 +1245,14 @@
       <c r="K4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1240,8 +1282,14 @@
       <c r="K5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1271,8 +1319,14 @@
       <c r="K6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1302,8 +1356,14 @@
       <c r="K7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1337,8 +1397,14 @@
       <c r="K8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1368,8 +1434,14 @@
       <c r="K9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1399,8 +1471,14 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1430,8 +1508,14 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1465,8 +1549,14 @@
       <c r="K12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1500,8 +1590,14 @@
       <c r="K13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1535,8 +1631,14 @@
       <c r="K14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1570,8 +1672,14 @@
       <c r="K15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1605,8 +1713,14 @@
       <c r="K16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1640,8 +1754,14 @@
       <c r="K17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1675,8 +1795,14 @@
       <c r="K18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1710,8 +1836,14 @@
       <c r="K19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1741,8 +1873,14 @@
       <c r="K20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1776,8 +1914,14 @@
       <c r="K21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1811,8 +1955,14 @@
       <c r="K22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1846,8 +1996,14 @@
       <c r="K23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1881,8 +2037,14 @@
       <c r="K24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1916,8 +2078,14 @@
       <c r="K25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1951,8 +2119,14 @@
       <c r="K26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1986,8 +2160,14 @@
       <c r="K27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2021,8 +2201,14 @@
       <c r="K28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2056,8 +2242,14 @@
       <c r="K29" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2077,22 +2269,28 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
         <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2112,22 +2310,28 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
       </c>
       <c r="K31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2157,8 +2361,14 @@
       <c r="K32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2192,8 +2402,14 @@
       <c r="K33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2227,8 +2443,14 @@
       <c r="K34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2262,8 +2484,14 @@
       <c r="K35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2297,8 +2525,14 @@
       <c r="K36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L36" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2332,8 +2566,14 @@
       <c r="K37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2367,8 +2607,14 @@
       <c r="K38" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -2402,8 +2648,14 @@
       <c r="K39" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -2437,8 +2689,14 @@
       <c r="K40" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L40" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -2472,8 +2730,14 @@
       <c r="K41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2507,8 +2771,14 @@
       <c r="K42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L42" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -2538,8 +2808,14 @@
       <c r="K43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -2569,8 +2845,14 @@
       <c r="K44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -2604,8 +2886,14 @@
       <c r="K45" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -2639,8 +2927,14 @@
       <c r="K46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L46" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -2674,8 +2968,14 @@
       <c r="K47" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -2709,8 +3009,14 @@
       <c r="K48" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -2744,8 +3050,14 @@
       <c r="K49" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -2779,8 +3091,14 @@
       <c r="K50" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -2814,8 +3132,14 @@
       <c r="K51" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2849,8 +3173,14 @@
       <c r="K52" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L52" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -2884,8 +3214,14 @@
       <c r="K53" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L53" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -2919,8 +3255,14 @@
       <c r="K54" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L54" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -2954,8 +3296,14 @@
       <c r="K55" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L55" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -2985,8 +3333,14 @@
       <c r="K56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -3016,8 +3370,14 @@
       <c r="K57" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -3051,8 +3411,14 @@
       <c r="K58" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L58" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -3086,8 +3452,14 @@
       <c r="K59" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L59" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -3121,8 +3493,14 @@
       <c r="K60" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L60" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3156,8 +3534,14 @@
       <c r="K61" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L61" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -3191,8 +3575,14 @@
       <c r="K62" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L62" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -3226,8 +3616,14 @@
       <c r="K63" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L63" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -3261,8 +3657,14 @@
       <c r="K64" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L64" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -3282,10 +3684,10 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -3294,10 +3696,16 @@
         <v>27</v>
       </c>
       <c r="K65" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -3331,8 +3739,14 @@
       <c r="K66" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L66" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -3366,8 +3780,14 @@
       <c r="K67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>89</v>
       </c>
@@ -3401,8 +3821,14 @@
       <c r="K68" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -3436,8 +3862,14 @@
       <c r="K69" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L69" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -3467,8 +3899,14 @@
       <c r="K70" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -3502,8 +3940,14 @@
       <c r="K71" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -3537,8 +3981,14 @@
       <c r="K72" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L72" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>94</v>
       </c>
@@ -3572,8 +4022,14 @@
       <c r="K73" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L73" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>95</v>
       </c>
@@ -3607,8 +4063,14 @@
       <c r="K74" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L74" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -3642,8 +4104,14 @@
       <c r="K75" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L75" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -3663,22 +4131,28 @@
         <v>19</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J76" t="s">
         <v>30</v>
       </c>
       <c r="K76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>98</v>
       </c>
@@ -3698,22 +4172,28 @@
         <v>29</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J77" t="s">
         <v>30</v>
       </c>
       <c r="K77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>100</v>
       </c>
@@ -3733,22 +4213,28 @@
         <v>29</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>3</v>
       </c>
       <c r="I78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J78" t="s">
         <v>30</v>
       </c>
       <c r="K78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>101</v>
       </c>
@@ -3768,22 +4254,28 @@
         <v>29</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H79">
         <v>1</v>
       </c>
       <c r="I79">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J79" t="s">
         <v>30</v>
       </c>
       <c r="K79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -3817,8 +4309,14 @@
       <c r="K80" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L80" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>103</v>
       </c>
@@ -3852,8 +4350,14 @@
       <c r="K81" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L81" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>104</v>
       </c>
@@ -3887,8 +4391,14 @@
       <c r="K82" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L82" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>105</v>
       </c>
@@ -3922,8 +4432,14 @@
       <c r="K83" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -3957,8 +4473,14 @@
       <c r="K84" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L84" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>107</v>
       </c>
@@ -3992,8 +4514,14 @@
       <c r="K85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L85" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>108</v>
       </c>
@@ -4023,8 +4551,14 @@
       <c r="K86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L86" s="1">
+        <v>0</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -4058,8 +4592,14 @@
       <c r="K87" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L87" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>110</v>
       </c>
@@ -4093,8 +4633,14 @@
       <c r="K88" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L88" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>111</v>
       </c>
@@ -4128,8 +4674,14 @@
       <c r="K89" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L89" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>112</v>
       </c>
@@ -4163,8 +4715,14 @@
       <c r="K90" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L90" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>113</v>
       </c>
@@ -4198,8 +4756,14 @@
       <c r="K91" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L91" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>114</v>
       </c>
@@ -4225,7 +4789,7 @@
         <v>1</v>
       </c>
       <c r="I92">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J92" t="s">
         <v>30</v>
@@ -4233,8 +4797,14 @@
       <c r="K92" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L92" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>115</v>
       </c>
@@ -4254,13 +4824,13 @@
         <v>37</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H93">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J93" t="s">
         <v>30</v>
@@ -4268,8 +4838,14 @@
       <c r="K93" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L93" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>116</v>
       </c>
@@ -4292,7 +4868,7 @@
         <v>1</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I94">
         <v>1</v>
@@ -4303,8 +4879,14 @@
       <c r="K94" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L94" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>117</v>
       </c>
@@ -4324,13 +4906,13 @@
         <v>29</v>
       </c>
       <c r="G95">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J95" t="s">
         <v>30</v>
@@ -4338,8 +4920,14 @@
       <c r="K95" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L95" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>118</v>
       </c>
@@ -4373,8 +4961,14 @@
       <c r="K96" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L96" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>119</v>
       </c>
@@ -4408,8 +5002,14 @@
       <c r="K97" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L97" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>120</v>
       </c>
@@ -4443,8 +5043,14 @@
       <c r="K98" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L98" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>121</v>
       </c>
@@ -4478,8 +5084,14 @@
       <c r="K99" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L99" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -4513,8 +5125,14 @@
       <c r="K100" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L100" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -4544,8 +5162,14 @@
       <c r="K101" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L101" s="1">
+        <v>0</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>124</v>
       </c>
@@ -4575,8 +5199,14 @@
       <c r="K102" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L102" s="1">
+        <v>0</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>125</v>
       </c>
@@ -4610,8 +5240,14 @@
       <c r="K103" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L103" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>126</v>
       </c>
@@ -4645,8 +5281,14 @@
       <c r="K104" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L104" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>127</v>
       </c>
@@ -4680,8 +5322,14 @@
       <c r="K105" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L105" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>128</v>
       </c>
@@ -4715,8 +5363,14 @@
       <c r="K106" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L106" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>129</v>
       </c>
@@ -4750,8 +5404,14 @@
       <c r="K107" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L107" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>130</v>
       </c>
@@ -4771,13 +5431,13 @@
         <v>29</v>
       </c>
       <c r="G108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H108">
         <v>3</v>
       </c>
       <c r="I108">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J108" t="s">
         <v>30</v>
@@ -4785,8 +5445,14 @@
       <c r="K108" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L108" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>131</v>
       </c>
@@ -4806,13 +5472,13 @@
         <v>37</v>
       </c>
       <c r="G109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J109" t="s">
         <v>30</v>
@@ -4820,8 +5486,14 @@
       <c r="K109" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L109" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>132</v>
       </c>
@@ -4841,13 +5513,13 @@
         <v>40</v>
       </c>
       <c r="G110">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I110">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J110" t="s">
         <v>30</v>
@@ -4855,8 +5527,14 @@
       <c r="K110" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L110" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>133</v>
       </c>
@@ -4876,13 +5554,13 @@
         <v>37</v>
       </c>
       <c r="G111">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H111">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I111">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J111" t="s">
         <v>30</v>
@@ -4890,8 +5568,14 @@
       <c r="K111" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L111" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>134</v>
       </c>
@@ -4911,10 +5595,10 @@
         <v>29</v>
       </c>
       <c r="G112">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I112">
         <v>1</v>
@@ -4925,8 +5609,14 @@
       <c r="K112" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L112" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>135</v>
       </c>
@@ -4960,8 +5650,14 @@
       <c r="K113" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L113" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>136</v>
       </c>
@@ -4995,8 +5691,14 @@
       <c r="K114" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L114" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>137</v>
       </c>
@@ -5030,8 +5732,14 @@
       <c r="K115" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L115" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>138</v>
       </c>
@@ -5065,8 +5773,14 @@
       <c r="K116" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L116" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>139</v>
       </c>
@@ -5100,8 +5814,14 @@
       <c r="K117" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L117" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>140</v>
       </c>
@@ -5131,8 +5851,14 @@
       <c r="K118" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L118" s="1">
+        <v>0</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>141</v>
       </c>
@@ -5162,8 +5888,14 @@
       <c r="K119" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L119" s="1">
+        <v>0</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>142</v>
       </c>
@@ -5197,8 +5929,14 @@
       <c r="K120" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L120" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>143</v>
       </c>
@@ -5232,8 +5970,14 @@
       <c r="K121" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L121" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>144</v>
       </c>
@@ -5267,8 +6011,14 @@
       <c r="K122" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L122" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>145</v>
       </c>
@@ -5302,8 +6052,14 @@
       <c r="K123" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L123" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>146</v>
       </c>
@@ -5337,8 +6093,14 @@
       <c r="K124" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L124" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>147</v>
       </c>
@@ -5372,8 +6134,14 @@
       <c r="K125" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L125" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>148</v>
       </c>
@@ -5407,8 +6175,14 @@
       <c r="K126" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L126" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>149</v>
       </c>
@@ -5428,10 +6202,10 @@
         <v>37</v>
       </c>
       <c r="G127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I127">
         <v>1</v>
@@ -5442,8 +6216,14 @@
       <c r="K127" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L127" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>150</v>
       </c>
@@ -5463,13 +6243,13 @@
         <v>29</v>
       </c>
       <c r="G128">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I128">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J128" t="s">
         <v>30</v>
@@ -5477,8 +6257,14 @@
       <c r="K128" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L128" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>151</v>
       </c>
@@ -5512,8 +6298,14 @@
       <c r="K129" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L129" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>152</v>
       </c>
@@ -5547,8 +6339,14 @@
       <c r="K130" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L130" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>153</v>
       </c>
@@ -5582,8 +6380,14 @@
       <c r="K131" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L131" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>154</v>
       </c>
@@ -5617,8 +6421,14 @@
       <c r="K132" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L132" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>155</v>
       </c>
@@ -5652,8 +6462,14 @@
       <c r="K133" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L133" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>156</v>
       </c>
@@ -5683,8 +6499,14 @@
       <c r="K134" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L134" s="1">
+        <v>0</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>157</v>
       </c>
@@ -5718,8 +6540,14 @@
       <c r="K135" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L135" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>158</v>
       </c>
@@ -5753,8 +6581,14 @@
       <c r="K136" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L136" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>159</v>
       </c>
@@ -5788,8 +6622,14 @@
       <c r="K137" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L137" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>160</v>
       </c>
@@ -5823,8 +6663,14 @@
       <c r="K138" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L138" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>161</v>
       </c>
@@ -5858,8 +6704,14 @@
       <c r="K139" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L139" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>162</v>
       </c>
@@ -5893,8 +6745,14 @@
       <c r="K140" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L140" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>163</v>
       </c>
@@ -5914,13 +6772,13 @@
         <v>29</v>
       </c>
       <c r="G141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H141">
         <v>1</v>
       </c>
       <c r="I141">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J141" t="s">
         <v>30</v>
@@ -5928,8 +6786,14 @@
       <c r="K141" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L141" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>164</v>
       </c>
@@ -5949,13 +6813,13 @@
         <v>29</v>
       </c>
       <c r="G142">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H142">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J142" t="s">
         <v>30</v>
@@ -5963,8 +6827,14 @@
       <c r="K142" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L142" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>165</v>
       </c>
@@ -5984,10 +6854,10 @@
         <v>29</v>
       </c>
       <c r="G143">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H143">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I143">
         <v>1</v>
@@ -5998,8 +6868,14 @@
       <c r="K143" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L143" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>166</v>
       </c>
@@ -6033,8 +6909,14 @@
       <c r="K144" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L144" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>167</v>
       </c>
@@ -6068,8 +6950,14 @@
       <c r="K145" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L145" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>168</v>
       </c>
@@ -6103,8 +6991,14 @@
       <c r="K146" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L146" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>169</v>
       </c>
@@ -6138,8 +7032,14 @@
       <c r="K147" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L147" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>170</v>
       </c>
@@ -6173,8 +7073,14 @@
       <c r="K148" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L148" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>171</v>
       </c>
@@ -6208,8 +7114,14 @@
       <c r="K149" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L149" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>172</v>
       </c>
@@ -6239,8 +7151,14 @@
       <c r="K150" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L150" s="1">
+        <v>0</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>173</v>
       </c>
@@ -6274,8 +7192,14 @@
       <c r="K151" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L151" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>174</v>
       </c>
@@ -6309,8 +7233,14 @@
       <c r="K152" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L152" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>175</v>
       </c>
@@ -6344,8 +7274,14 @@
       <c r="K153" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L153" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>176</v>
       </c>
@@ -6379,8 +7315,14 @@
       <c r="K154" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L154" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>177</v>
       </c>
@@ -6414,8 +7356,14 @@
       <c r="K155" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L155" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>178</v>
       </c>
@@ -6449,8 +7397,14 @@
       <c r="K156" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L156" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>179</v>
       </c>
@@ -6484,8 +7438,14 @@
       <c r="K157" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L157" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>180</v>
       </c>
@@ -6519,8 +7479,14 @@
       <c r="K158" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L158" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>181</v>
       </c>
@@ -6554,8 +7520,14 @@
       <c r="K159" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L159" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>182</v>
       </c>
@@ -6589,8 +7561,14 @@
       <c r="K160" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L160" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M160" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>183</v>
       </c>
@@ -6624,8 +7602,14 @@
       <c r="K161" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L161" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M161" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>184</v>
       </c>
@@ -6659,8 +7643,14 @@
       <c r="K162" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L162" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>185</v>
       </c>
@@ -6690,8 +7680,14 @@
       <c r="K163" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L163" s="1">
+        <v>0</v>
+      </c>
+      <c r="M163" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>186</v>
       </c>
@@ -6721,8 +7717,14 @@
       <c r="K164" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L164" s="1">
+        <v>0</v>
+      </c>
+      <c r="M164" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>187</v>
       </c>
@@ -6756,8 +7758,14 @@
       <c r="K165" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L165" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M165" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>188</v>
       </c>
@@ -6791,8 +7799,14 @@
       <c r="K166" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L166" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>189</v>
       </c>
@@ -6826,8 +7840,14 @@
       <c r="K167" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L167" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M167" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>190</v>
       </c>
@@ -6861,8 +7881,14 @@
       <c r="K168" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L168" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M168" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>191</v>
       </c>
@@ -6896,8 +7922,14 @@
       <c r="K169" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L169" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M169" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>192</v>
       </c>
@@ -6931,8 +7963,14 @@
       <c r="K170" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L170" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M170" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>193</v>
       </c>
@@ -6966,8 +8004,14 @@
       <c r="K171" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L171" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>194</v>
       </c>
@@ -7001,8 +8045,14 @@
       <c r="K172" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L172" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M172" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>195</v>
       </c>
@@ -7036,8 +8086,14 @@
       <c r="K173" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L173" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M173" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>196</v>
       </c>
@@ -7071,8 +8127,14 @@
       <c r="K174" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L174" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>197</v>
       </c>
@@ -7106,8 +8168,14 @@
       <c r="K175" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L175" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M175" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>198</v>
       </c>
@@ -7137,8 +8205,14 @@
       <c r="K176" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L176" s="1">
+        <v>0</v>
+      </c>
+      <c r="M176" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>199</v>
       </c>
@@ -7168,8 +8242,14 @@
       <c r="K177" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L177" s="1">
+        <v>0</v>
+      </c>
+      <c r="M177" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>200</v>
       </c>
@@ -7203,8 +8283,14 @@
       <c r="K178" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L178" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M178" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>201</v>
       </c>
@@ -7238,8 +8324,14 @@
       <c r="K179" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L179" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M179" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>202</v>
       </c>
@@ -7273,8 +8365,14 @@
       <c r="K180" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L180" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M180" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>203</v>
       </c>
@@ -7308,8 +8406,14 @@
       <c r="K181" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L181" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M181" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>204</v>
       </c>
@@ -7343,8 +8447,14 @@
       <c r="K182" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L182" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M182" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>205</v>
       </c>
@@ -7378,8 +8488,14 @@
       <c r="K183" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L183" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M183" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>206</v>
       </c>
@@ -7413,8 +8529,14 @@
       <c r="K184" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L184" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M184" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>207</v>
       </c>
@@ -7448,8 +8570,14 @@
       <c r="K185" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L185" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M185" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>208</v>
       </c>
@@ -7483,8 +8611,14 @@
       <c r="K186" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L186" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M186" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>209</v>
       </c>
@@ -7518,8 +8652,14 @@
       <c r="K187" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L187" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M187" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>210</v>
       </c>
@@ -7549,8 +8689,14 @@
       <c r="K188" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L188" s="1">
+        <v>0</v>
+      </c>
+      <c r="M188" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>211</v>
       </c>
@@ -7584,8 +8730,14 @@
       <c r="K189" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L189" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M189" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -7619,8 +8771,14 @@
       <c r="K190" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L190" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M190" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>213</v>
       </c>
@@ -7654,8 +8812,14 @@
       <c r="K191" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L191" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M191" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>214</v>
       </c>
@@ -7689,8 +8853,14 @@
       <c r="K192" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L192" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M192" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>215</v>
       </c>
@@ -7724,8 +8894,14 @@
       <c r="K193" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L193" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M193" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>216</v>
       </c>
@@ -7759,8 +8935,14 @@
       <c r="K194" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L194" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M194" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>217</v>
       </c>
@@ -7794,8 +8976,14 @@
       <c r="K195" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L195" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M195" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>218</v>
       </c>
@@ -7829,8 +9017,14 @@
       <c r="K196" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L196" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M196" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>219</v>
       </c>
@@ -7864,8 +9058,14 @@
       <c r="K197" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L197" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M197" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>220</v>
       </c>
@@ -7899,8 +9099,14 @@
       <c r="K198" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L198" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M198" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>221</v>
       </c>
@@ -7934,8 +9140,14 @@
       <c r="K199" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L199" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M199" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>222</v>
       </c>
@@ -7965,8 +9177,14 @@
       <c r="K200" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L200" s="1">
+        <v>0</v>
+      </c>
+      <c r="M200" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>223</v>
       </c>
@@ -8000,8 +9218,14 @@
       <c r="K201" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L201" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M201" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>224</v>
       </c>
@@ -8035,8 +9259,14 @@
       <c r="K202" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L202" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M202" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>225</v>
       </c>
@@ -8070,8 +9300,14 @@
       <c r="K203" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L203" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M203" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>226</v>
       </c>
@@ -8105,8 +9341,14 @@
       <c r="K204" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L204" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M204" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>227</v>
       </c>
@@ -8140,8 +9382,14 @@
       <c r="K205" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L205" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M205" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>228</v>
       </c>
@@ -8175,8 +9423,14 @@
       <c r="K206" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L206" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M206" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>229</v>
       </c>
@@ -8210,8 +9464,14 @@
       <c r="K207" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L207" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M207" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>230</v>
       </c>
@@ -8245,8 +9505,14 @@
       <c r="K208" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L208" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M208" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>231</v>
       </c>
@@ -8276,8 +9542,14 @@
       <c r="K209" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L209" s="1">
+        <v>0</v>
+      </c>
+      <c r="M209" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>232</v>
       </c>
@@ -8307,8 +9579,14 @@
       <c r="K210" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L210" s="1">
+        <v>0</v>
+      </c>
+      <c r="M210" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>233</v>
       </c>
@@ -8338,8 +9616,14 @@
       <c r="K211" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L211" s="1">
+        <v>0</v>
+      </c>
+      <c r="M211" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>234</v>
       </c>
@@ -8373,8 +9657,14 @@
       <c r="K212" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L212" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M212" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>235</v>
       </c>
@@ -8404,8 +9694,14 @@
       <c r="K213" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L213" s="1">
+        <v>0</v>
+      </c>
+      <c r="M213" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>236</v>
       </c>
@@ -8435,8 +9731,14 @@
       <c r="K214" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L214" s="1">
+        <v>0</v>
+      </c>
+      <c r="M214" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>237</v>
       </c>
@@ -8466,8 +9768,14 @@
       <c r="K215" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L215" s="1">
+        <v>0</v>
+      </c>
+      <c r="M215" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>238</v>
       </c>
@@ -8501,8 +9809,14 @@
       <c r="K216" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L216" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M216" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>239</v>
       </c>
@@ -8532,8 +9846,14 @@
       <c r="K217" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L217" s="1">
+        <v>0</v>
+      </c>
+      <c r="M217" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>240</v>
       </c>
@@ -8562,6 +9882,12 @@
       </c>
       <c r="K218" t="s">
         <v>13</v>
+      </c>
+      <c r="L218" s="1">
+        <v>0</v>
+      </c>
+      <c r="M218" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
az előző még mindig szar volt, na de most!
</commit_message>
<xml_diff>
--- a/resources/terkep_adatok.xlsx
+++ b/resources/terkep_adatok.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="242">
   <si>
     <t>Koordináta</t>
   </si>
@@ -742,21 +742,6 @@
   </si>
   <si>
     <t>Q9</t>
-  </si>
-  <si>
-    <t>Fegyver típus</t>
-  </si>
-  <si>
-    <t>Maula Pistol</t>
-  </si>
-  <si>
-    <t>Crysknife</t>
-  </si>
-  <si>
-    <t>Lasgun</t>
-  </si>
-  <si>
-    <t>koordináta</t>
   </si>
   <si>
     <t>lc</t>
@@ -1085,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M218"/>
+  <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="N204" sqref="N204"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1096,7 +1081,7 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,14 +1115,8 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1167,14 +1146,8 @@
       <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1204,14 +1177,8 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1245,14 +1212,8 @@
       <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1282,14 +1243,8 @@
       <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1319,14 +1274,8 @@
       <c r="K6" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1356,14 +1305,8 @@
       <c r="K7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1397,14 +1340,8 @@
       <c r="K8" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1434,14 +1371,8 @@
       <c r="K9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1471,14 +1402,8 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1508,14 +1433,8 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1549,14 +1468,8 @@
       <c r="K12" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1590,14 +1503,8 @@
       <c r="K13" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1631,14 +1538,8 @@
       <c r="K14" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1672,14 +1573,8 @@
       <c r="K15" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1713,14 +1608,8 @@
       <c r="K16" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1754,14 +1643,8 @@
       <c r="K17" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1795,14 +1678,8 @@
       <c r="K18" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1836,14 +1713,8 @@
       <c r="K19" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1873,14 +1744,8 @@
       <c r="K20" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="1">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1914,14 +1779,8 @@
       <c r="K21" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1955,14 +1814,8 @@
       <c r="K22" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1996,14 +1849,8 @@
       <c r="K23" t="s">
         <v>28</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2037,14 +1884,8 @@
       <c r="K24" t="s">
         <v>17</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2078,14 +1919,8 @@
       <c r="K25" t="s">
         <v>17</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2119,14 +1954,8 @@
       <c r="K26" t="s">
         <v>46</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2160,14 +1989,8 @@
       <c r="K27" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2201,14 +2024,8 @@
       <c r="K28" t="s">
         <v>22</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2242,14 +2059,8 @@
       <c r="K29" t="s">
         <v>37</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2283,14 +2094,8 @@
       <c r="K30" t="s">
         <v>40</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2324,14 +2129,8 @@
       <c r="K31" t="s">
         <v>40</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2361,14 +2160,8 @@
       <c r="K32" t="s">
         <v>13</v>
       </c>
-      <c r="L32" s="1">
-        <v>0</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2402,14 +2195,8 @@
       <c r="K33" t="s">
         <v>40</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2443,14 +2230,8 @@
       <c r="K34" t="s">
         <v>40</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2484,14 +2265,8 @@
       <c r="K35" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2525,14 +2300,8 @@
       <c r="K36" t="s">
         <v>17</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2566,14 +2335,8 @@
       <c r="K37" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2607,14 +2370,8 @@
       <c r="K38" t="s">
         <v>22</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -2648,14 +2405,8 @@
       <c r="K39" t="s">
         <v>22</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -2689,14 +2440,8 @@
       <c r="K40" t="s">
         <v>37</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -2730,14 +2475,8 @@
       <c r="K41" t="s">
         <v>40</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2771,14 +2510,8 @@
       <c r="K42" t="s">
         <v>40</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -2808,14 +2541,8 @@
       <c r="K43" t="s">
         <v>13</v>
       </c>
-      <c r="L43" s="1">
-        <v>0</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -2845,14 +2572,8 @@
       <c r="K44" t="s">
         <v>13</v>
       </c>
-      <c r="L44" s="1">
-        <v>0</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -2886,14 +2607,8 @@
       <c r="K45" t="s">
         <v>40</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -2927,14 +2642,8 @@
       <c r="K46" t="s">
         <v>40</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -2968,14 +2677,8 @@
       <c r="K47" t="s">
         <v>40</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -3009,14 +2712,8 @@
       <c r="K48" t="s">
         <v>28</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -3050,14 +2747,8 @@
       <c r="K49" t="s">
         <v>17</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -3091,14 +2782,8 @@
       <c r="K50" t="s">
         <v>46</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -3132,14 +2817,8 @@
       <c r="K51" t="s">
         <v>22</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -3173,14 +2852,8 @@
       <c r="K52" t="s">
         <v>37</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -3214,14 +2887,8 @@
       <c r="K53" t="s">
         <v>40</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -3255,14 +2922,8 @@
       <c r="K54" t="s">
         <v>40</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -3296,14 +2957,8 @@
       <c r="K55" t="s">
         <v>40</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -3333,14 +2988,8 @@
       <c r="K56" t="s">
         <v>13</v>
       </c>
-      <c r="L56" s="1">
-        <v>0</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -3370,14 +3019,8 @@
       <c r="K57" t="s">
         <v>13</v>
       </c>
-      <c r="L57" s="1">
-        <v>0</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -3411,14 +3054,8 @@
       <c r="K58" t="s">
         <v>22</v>
       </c>
-      <c r="L58" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -3452,14 +3089,8 @@
       <c r="K59" t="s">
         <v>37</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -3493,14 +3124,8 @@
       <c r="K60" t="s">
         <v>40</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3534,14 +3159,8 @@
       <c r="K61" t="s">
         <v>40</v>
       </c>
-      <c r="L61" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -3575,14 +3194,8 @@
       <c r="K62" t="s">
         <v>28</v>
       </c>
-      <c r="L62" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -3616,14 +3229,8 @@
       <c r="K63" t="s">
         <v>17</v>
       </c>
-      <c r="L63" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -3657,14 +3264,8 @@
       <c r="K64" t="s">
         <v>22</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -3696,16 +3297,10 @@
         <v>27</v>
       </c>
       <c r="K65" t="s">
-        <v>246</v>
-      </c>
-      <c r="L65" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M65" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -3739,14 +3334,8 @@
       <c r="K66" t="s">
         <v>40</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -3780,14 +3369,8 @@
       <c r="K67" t="s">
         <v>40</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M67" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>89</v>
       </c>
@@ -3821,14 +3404,8 @@
       <c r="K68" t="s">
         <v>28</v>
       </c>
-      <c r="L68" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -3862,14 +3439,8 @@
       <c r="K69" t="s">
         <v>17</v>
       </c>
-      <c r="L69" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M69" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -3899,14 +3470,8 @@
       <c r="K70" t="s">
         <v>13</v>
       </c>
-      <c r="L70" s="1">
-        <v>0</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -3940,14 +3505,8 @@
       <c r="K71" t="s">
         <v>22</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -3981,14 +3540,8 @@
       <c r="K72" t="s">
         <v>22</v>
       </c>
-      <c r="L72" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>94</v>
       </c>
@@ -4022,14 +3575,8 @@
       <c r="K73" t="s">
         <v>22</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M73" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>95</v>
       </c>
@@ -4063,14 +3610,8 @@
       <c r="K74" t="s">
         <v>22</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M74" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -4090,10 +3631,10 @@
         <v>11</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -4102,16 +3643,10 @@
         <v>30</v>
       </c>
       <c r="K75" t="s">
-        <v>46</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -4145,14 +3680,8 @@
       <c r="K76" t="s">
         <v>40</v>
       </c>
-      <c r="L76" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M76" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>98</v>
       </c>
@@ -4186,14 +3715,8 @@
       <c r="K77" t="s">
         <v>40</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>100</v>
       </c>
@@ -4227,14 +3750,8 @@
       <c r="K78" t="s">
         <v>17</v>
       </c>
-      <c r="L78" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>101</v>
       </c>
@@ -4268,14 +3785,8 @@
       <c r="K79" t="s">
         <v>22</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -4309,14 +3820,8 @@
       <c r="K80" t="s">
         <v>40</v>
       </c>
-      <c r="L80" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>103</v>
       </c>
@@ -4350,14 +3855,8 @@
       <c r="K81" t="s">
         <v>28</v>
       </c>
-      <c r="L81" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M81" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>104</v>
       </c>
@@ -4391,14 +3890,8 @@
       <c r="K82" t="s">
         <v>17</v>
       </c>
-      <c r="L82" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>105</v>
       </c>
@@ -4432,14 +3925,8 @@
       <c r="K83" t="s">
         <v>17</v>
       </c>
-      <c r="L83" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -4473,14 +3960,8 @@
       <c r="K84" t="s">
         <v>17</v>
       </c>
-      <c r="L84" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M84" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>107</v>
       </c>
@@ -4514,14 +3995,8 @@
       <c r="K85" t="s">
         <v>17</v>
       </c>
-      <c r="L85" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>108</v>
       </c>
@@ -4551,14 +4026,8 @@
       <c r="K86" t="s">
         <v>13</v>
       </c>
-      <c r="L86" s="1">
-        <v>0</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -4592,14 +4061,8 @@
       <c r="K87" t="s">
         <v>22</v>
       </c>
-      <c r="L87" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>110</v>
       </c>
@@ -4633,14 +4096,8 @@
       <c r="K88" t="s">
         <v>22</v>
       </c>
-      <c r="L88" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>111</v>
       </c>
@@ -4674,14 +4131,8 @@
       <c r="K89" t="s">
         <v>22</v>
       </c>
-      <c r="L89" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>112</v>
       </c>
@@ -4715,14 +4166,8 @@
       <c r="K90" t="s">
         <v>22</v>
       </c>
-      <c r="L90" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M90" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>113</v>
       </c>
@@ -4756,14 +4201,8 @@
       <c r="K91" t="s">
         <v>22</v>
       </c>
-      <c r="L91" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>114</v>
       </c>
@@ -4797,14 +4236,8 @@
       <c r="K92" t="s">
         <v>99</v>
       </c>
-      <c r="L92" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>115</v>
       </c>
@@ -4838,14 +4271,8 @@
       <c r="K93" t="s">
         <v>99</v>
       </c>
-      <c r="L93" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>116</v>
       </c>
@@ -4879,14 +4306,8 @@
       <c r="K94" t="s">
         <v>99</v>
       </c>
-      <c r="L94" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M94" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>117</v>
       </c>
@@ -4920,14 +4341,8 @@
       <c r="K95" t="s">
         <v>99</v>
       </c>
-      <c r="L95" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M95" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>118</v>
       </c>
@@ -4961,14 +4376,8 @@
       <c r="K96" t="s">
         <v>17</v>
       </c>
-      <c r="L96" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M96" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>119</v>
       </c>
@@ -5002,14 +4411,8 @@
       <c r="K97" t="s">
         <v>17</v>
       </c>
-      <c r="L97" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M97" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>120</v>
       </c>
@@ -5043,14 +4446,8 @@
       <c r="K98" t="s">
         <v>17</v>
       </c>
-      <c r="L98" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M98" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>121</v>
       </c>
@@ -5084,14 +4481,8 @@
       <c r="K99" t="s">
         <v>17</v>
       </c>
-      <c r="L99" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M99" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -5125,14 +4516,8 @@
       <c r="K100" t="s">
         <v>17</v>
       </c>
-      <c r="L100" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -5162,14 +4547,8 @@
       <c r="K101" t="s">
         <v>13</v>
       </c>
-      <c r="L101" s="1">
-        <v>0</v>
-      </c>
-      <c r="M101" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>124</v>
       </c>
@@ -5199,14 +4578,8 @@
       <c r="K102" t="s">
         <v>13</v>
       </c>
-      <c r="L102" s="1">
-        <v>0</v>
-      </c>
-      <c r="M102" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>125</v>
       </c>
@@ -5240,14 +4613,8 @@
       <c r="K103" t="s">
         <v>46</v>
       </c>
-      <c r="L103" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M103" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>126</v>
       </c>
@@ -5281,14 +4648,8 @@
       <c r="K104" t="s">
         <v>46</v>
       </c>
-      <c r="L104" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>127</v>
       </c>
@@ -5322,14 +4683,8 @@
       <c r="K105" t="s">
         <v>46</v>
       </c>
-      <c r="L105" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M105" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>128</v>
       </c>
@@ -5363,14 +4718,8 @@
       <c r="K106" t="s">
         <v>46</v>
       </c>
-      <c r="L106" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M106" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>129</v>
       </c>
@@ -5404,14 +4753,8 @@
       <c r="K107" t="s">
         <v>46</v>
       </c>
-      <c r="L107" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M107" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>130</v>
       </c>
@@ -5445,14 +4788,8 @@
       <c r="K108" t="s">
         <v>99</v>
       </c>
-      <c r="L108" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>131</v>
       </c>
@@ -5486,14 +4823,8 @@
       <c r="K109" t="s">
         <v>99</v>
       </c>
-      <c r="L109" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M109" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>132</v>
       </c>
@@ -5527,14 +4858,8 @@
       <c r="K110" t="s">
         <v>99</v>
       </c>
-      <c r="L110" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M110" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>133</v>
       </c>
@@ -5568,14 +4893,8 @@
       <c r="K111" t="s">
         <v>99</v>
       </c>
-      <c r="L111" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M111" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>134</v>
       </c>
@@ -5609,14 +4928,8 @@
       <c r="K112" t="s">
         <v>99</v>
       </c>
-      <c r="L112" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M112" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>135</v>
       </c>
@@ -5650,14 +4963,8 @@
       <c r="K113" t="s">
         <v>46</v>
       </c>
-      <c r="L113" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M113" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>136</v>
       </c>
@@ -5691,14 +4998,8 @@
       <c r="K114" t="s">
         <v>46</v>
       </c>
-      <c r="L114" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M114" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>137</v>
       </c>
@@ -5732,14 +5033,8 @@
       <c r="K115" t="s">
         <v>46</v>
       </c>
-      <c r="L115" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>138</v>
       </c>
@@ -5773,14 +5068,8 @@
       <c r="K116" t="s">
         <v>46</v>
       </c>
-      <c r="L116" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M116" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>139</v>
       </c>
@@ -5814,14 +5103,8 @@
       <c r="K117" t="s">
         <v>46</v>
       </c>
-      <c r="L117" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M117" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>140</v>
       </c>
@@ -5851,14 +5134,8 @@
       <c r="K118" t="s">
         <v>13</v>
       </c>
-      <c r="L118" s="1">
-        <v>0</v>
-      </c>
-      <c r="M118" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>141</v>
       </c>
@@ -5888,14 +5165,8 @@
       <c r="K119" t="s">
         <v>13</v>
       </c>
-      <c r="L119" s="1">
-        <v>0</v>
-      </c>
-      <c r="M119" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>142</v>
       </c>
@@ -5929,14 +5200,8 @@
       <c r="K120" t="s">
         <v>17</v>
       </c>
-      <c r="L120" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M120" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>143</v>
       </c>
@@ -5970,14 +5235,8 @@
       <c r="K121" t="s">
         <v>17</v>
       </c>
-      <c r="L121" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M121" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>144</v>
       </c>
@@ -6011,14 +5270,8 @@
       <c r="K122" t="s">
         <v>17</v>
       </c>
-      <c r="L122" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M122" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>145</v>
       </c>
@@ -6052,14 +5305,8 @@
       <c r="K123" t="s">
         <v>17</v>
       </c>
-      <c r="L123" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M123" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>146</v>
       </c>
@@ -6093,14 +5340,8 @@
       <c r="K124" t="s">
         <v>17</v>
       </c>
-      <c r="L124" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M124" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>147</v>
       </c>
@@ -6134,14 +5375,8 @@
       <c r="K125" t="s">
         <v>99</v>
       </c>
-      <c r="L125" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M125" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>148</v>
       </c>
@@ -6175,14 +5410,8 @@
       <c r="K126" t="s">
         <v>99</v>
       </c>
-      <c r="L126" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M126" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>149</v>
       </c>
@@ -6216,14 +5445,8 @@
       <c r="K127" t="s">
         <v>99</v>
       </c>
-      <c r="L127" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M127" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>150</v>
       </c>
@@ -6257,14 +5480,8 @@
       <c r="K128" t="s">
         <v>99</v>
       </c>
-      <c r="L128" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M128" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>151</v>
       </c>
@@ -6298,14 +5515,8 @@
       <c r="K129" t="s">
         <v>22</v>
       </c>
-      <c r="L129" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M129" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>152</v>
       </c>
@@ -6339,14 +5550,8 @@
       <c r="K130" t="s">
         <v>22</v>
       </c>
-      <c r="L130" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M130" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>153</v>
       </c>
@@ -6380,14 +5585,8 @@
       <c r="K131" t="s">
         <v>22</v>
       </c>
-      <c r="L131" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M131" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>154</v>
       </c>
@@ -6421,14 +5620,8 @@
       <c r="K132" t="s">
         <v>22</v>
       </c>
-      <c r="L132" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M132" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>155</v>
       </c>
@@ -6462,14 +5655,8 @@
       <c r="K133" t="s">
         <v>22</v>
       </c>
-      <c r="L133" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M133" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>156</v>
       </c>
@@ -6499,14 +5686,8 @@
       <c r="K134" t="s">
         <v>13</v>
       </c>
-      <c r="L134" s="1">
-        <v>0</v>
-      </c>
-      <c r="M134" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>157</v>
       </c>
@@ -6540,14 +5721,8 @@
       <c r="K135" t="s">
         <v>17</v>
       </c>
-      <c r="L135" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M135" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>158</v>
       </c>
@@ -6581,14 +5756,8 @@
       <c r="K136" t="s">
         <v>17</v>
       </c>
-      <c r="L136" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M136" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>159</v>
       </c>
@@ -6622,14 +5791,8 @@
       <c r="K137" t="s">
         <v>17</v>
       </c>
-      <c r="L137" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M137" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>160</v>
       </c>
@@ -6663,14 +5826,8 @@
       <c r="K138" t="s">
         <v>17</v>
       </c>
-      <c r="L138" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>161</v>
       </c>
@@ -6704,14 +5861,8 @@
       <c r="K139" t="s">
         <v>28</v>
       </c>
-      <c r="L139" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M139" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>162</v>
       </c>
@@ -6745,14 +5896,8 @@
       <c r="K140" t="s">
         <v>40</v>
       </c>
-      <c r="L140" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M140" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>163</v>
       </c>
@@ -6786,14 +5931,8 @@
       <c r="K141" t="s">
         <v>99</v>
       </c>
-      <c r="L141" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M141" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>164</v>
       </c>
@@ -6827,14 +5966,8 @@
       <c r="K142" t="s">
         <v>99</v>
       </c>
-      <c r="L142" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M142" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>165</v>
       </c>
@@ -6868,14 +6001,8 @@
       <c r="K143" t="s">
         <v>99</v>
       </c>
-      <c r="L143" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M143" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>166</v>
       </c>
@@ -6909,14 +6036,8 @@
       <c r="K144" t="s">
         <v>40</v>
       </c>
-      <c r="L144" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M144" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>167</v>
       </c>
@@ -6950,14 +6071,8 @@
       <c r="K145" t="s">
         <v>37</v>
       </c>
-      <c r="L145" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M145" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>168</v>
       </c>
@@ -6991,14 +6106,8 @@
       <c r="K146" t="s">
         <v>22</v>
       </c>
-      <c r="L146" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M146" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>169</v>
       </c>
@@ -7032,14 +6141,8 @@
       <c r="K147" t="s">
         <v>22</v>
       </c>
-      <c r="L147" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M147" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>170</v>
       </c>
@@ -7073,14 +6176,8 @@
       <c r="K148" t="s">
         <v>22</v>
       </c>
-      <c r="L148" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M148" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>171</v>
       </c>
@@ -7100,13 +6197,13 @@
         <v>0</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I149">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J149" t="s">
         <v>16</v>
@@ -7114,14 +6211,8 @@
       <c r="K149" t="s">
         <v>13</v>
       </c>
-      <c r="L149" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M149" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>172</v>
       </c>
@@ -7151,14 +6242,8 @@
       <c r="K150" t="s">
         <v>13</v>
       </c>
-      <c r="L150" s="1">
-        <v>0</v>
-      </c>
-      <c r="M150" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>173</v>
       </c>
@@ -7192,14 +6277,8 @@
       <c r="K151" t="s">
         <v>17</v>
       </c>
-      <c r="L151" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M151" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>174</v>
       </c>
@@ -7233,14 +6312,8 @@
       <c r="K152" t="s">
         <v>28</v>
       </c>
-      <c r="L152" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M152" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>175</v>
       </c>
@@ -7274,14 +6347,8 @@
       <c r="K153" t="s">
         <v>40</v>
       </c>
-      <c r="L153" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M153" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>176</v>
       </c>
@@ -7315,14 +6382,8 @@
       <c r="K154" t="s">
         <v>40</v>
       </c>
-      <c r="L154" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M154" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>177</v>
       </c>
@@ -7356,14 +6417,8 @@
       <c r="K155" t="s">
         <v>37</v>
       </c>
-      <c r="L155" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M155" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>178</v>
       </c>
@@ -7397,14 +6452,8 @@
       <c r="K156" t="s">
         <v>22</v>
       </c>
-      <c r="L156" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M156" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>179</v>
       </c>
@@ -7438,14 +6487,8 @@
       <c r="K157" t="s">
         <v>17</v>
       </c>
-      <c r="L157" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M157" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>180</v>
       </c>
@@ -7479,14 +6522,8 @@
       <c r="K158" t="s">
         <v>28</v>
       </c>
-      <c r="L158" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M158" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>181</v>
       </c>
@@ -7520,14 +6557,8 @@
       <c r="K159" t="s">
         <v>40</v>
       </c>
-      <c r="L159" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M159" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>182</v>
       </c>
@@ -7561,14 +6592,8 @@
       <c r="K160" t="s">
         <v>40</v>
       </c>
-      <c r="L160" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M160" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>183</v>
       </c>
@@ -7602,14 +6627,8 @@
       <c r="K161" t="s">
         <v>37</v>
       </c>
-      <c r="L161" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M161" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>184</v>
       </c>
@@ -7643,14 +6662,8 @@
       <c r="K162" t="s">
         <v>22</v>
       </c>
-      <c r="L162" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M162" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>185</v>
       </c>
@@ -7680,14 +6693,8 @@
       <c r="K163" t="s">
         <v>13</v>
       </c>
-      <c r="L163" s="1">
-        <v>0</v>
-      </c>
-      <c r="M163" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>186</v>
       </c>
@@ -7717,14 +6724,8 @@
       <c r="K164" t="s">
         <v>13</v>
       </c>
-      <c r="L164" s="1">
-        <v>0</v>
-      </c>
-      <c r="M164" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>187</v>
       </c>
@@ -7758,14 +6759,8 @@
       <c r="K165" t="s">
         <v>40</v>
       </c>
-      <c r="L165" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M165" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>188</v>
       </c>
@@ -7799,14 +6794,8 @@
       <c r="K166" t="s">
         <v>40</v>
       </c>
-      <c r="L166" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M166" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>189</v>
       </c>
@@ -7840,14 +6829,8 @@
       <c r="K167" t="s">
         <v>40</v>
       </c>
-      <c r="L167" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M167" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>190</v>
       </c>
@@ -7881,14 +6864,8 @@
       <c r="K168" t="s">
         <v>37</v>
       </c>
-      <c r="L168" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M168" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>191</v>
       </c>
@@ -7922,14 +6899,8 @@
       <c r="K169" t="s">
         <v>22</v>
       </c>
-      <c r="L169" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M169" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>192</v>
       </c>
@@ -7963,14 +6934,8 @@
       <c r="K170" t="s">
         <v>46</v>
       </c>
-      <c r="L170" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M170" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>193</v>
       </c>
@@ -8004,14 +6969,8 @@
       <c r="K171" t="s">
         <v>17</v>
       </c>
-      <c r="L171" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M171" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>194</v>
       </c>
@@ -8045,14 +7004,8 @@
       <c r="K172" t="s">
         <v>28</v>
       </c>
-      <c r="L172" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M172" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>195</v>
       </c>
@@ -8086,14 +7039,8 @@
       <c r="K173" t="s">
         <v>40</v>
       </c>
-      <c r="L173" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M173" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>196</v>
       </c>
@@ -8127,14 +7074,8 @@
       <c r="K174" t="s">
         <v>40</v>
       </c>
-      <c r="L174" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M174" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>197</v>
       </c>
@@ -8168,14 +7109,8 @@
       <c r="K175" t="s">
         <v>40</v>
       </c>
-      <c r="L175" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M175" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>198</v>
       </c>
@@ -8205,14 +7140,8 @@
       <c r="K176" t="s">
         <v>13</v>
       </c>
-      <c r="L176" s="1">
-        <v>0</v>
-      </c>
-      <c r="M176" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>199</v>
       </c>
@@ -8242,14 +7171,8 @@
       <c r="K177" t="s">
         <v>13</v>
       </c>
-      <c r="L177" s="1">
-        <v>0</v>
-      </c>
-      <c r="M177" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>200</v>
       </c>
@@ -8283,14 +7206,8 @@
       <c r="K178" t="s">
         <v>40</v>
       </c>
-      <c r="L178" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M178" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>201</v>
       </c>
@@ -8324,14 +7241,8 @@
       <c r="K179" t="s">
         <v>40</v>
       </c>
-      <c r="L179" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M179" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>202</v>
       </c>
@@ -8365,14 +7276,8 @@
       <c r="K180" t="s">
         <v>37</v>
       </c>
-      <c r="L180" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M180" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>203</v>
       </c>
@@ -8406,14 +7311,8 @@
       <c r="K181" t="s">
         <v>22</v>
       </c>
-      <c r="L181" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M181" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>204</v>
       </c>
@@ -8447,14 +7346,8 @@
       <c r="K182" t="s">
         <v>22</v>
       </c>
-      <c r="L182" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M182" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>205</v>
       </c>
@@ -8488,14 +7381,8 @@
       <c r="K183" t="s">
         <v>17</v>
       </c>
-      <c r="L183" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M183" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>206</v>
       </c>
@@ -8529,14 +7416,8 @@
       <c r="K184" t="s">
         <v>17</v>
       </c>
-      <c r="L184" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M184" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>207</v>
       </c>
@@ -8570,14 +7451,8 @@
       <c r="K185" t="s">
         <v>28</v>
       </c>
-      <c r="L185" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M185" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>208</v>
       </c>
@@ -8611,14 +7486,8 @@
       <c r="K186" t="s">
         <v>40</v>
       </c>
-      <c r="L186" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M186" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>209</v>
       </c>
@@ -8652,14 +7521,8 @@
       <c r="K187" t="s">
         <v>40</v>
       </c>
-      <c r="L187" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M187" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>210</v>
       </c>
@@ -8689,14 +7552,8 @@
       <c r="K188" t="s">
         <v>13</v>
       </c>
-      <c r="L188" s="1">
-        <v>0</v>
-      </c>
-      <c r="M188" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>211</v>
       </c>
@@ -8730,14 +7587,8 @@
       <c r="K189" t="s">
         <v>40</v>
       </c>
-      <c r="L189" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M189" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -8771,14 +7622,8 @@
       <c r="K190" t="s">
         <v>40</v>
       </c>
-      <c r="L190" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M190" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>213</v>
       </c>
@@ -8812,14 +7657,8 @@
       <c r="K191" t="s">
         <v>37</v>
       </c>
-      <c r="L191" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M191" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>214</v>
       </c>
@@ -8853,14 +7692,8 @@
       <c r="K192" t="s">
         <v>22</v>
       </c>
-      <c r="L192" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M192" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>215</v>
       </c>
@@ -8894,14 +7727,8 @@
       <c r="K193" t="s">
         <v>22</v>
       </c>
-      <c r="L193" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M193" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>216</v>
       </c>
@@ -8935,14 +7762,8 @@
       <c r="K194" t="s">
         <v>46</v>
       </c>
-      <c r="L194" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M194" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>217</v>
       </c>
@@ -8976,14 +7797,8 @@
       <c r="K195" t="s">
         <v>17</v>
       </c>
-      <c r="L195" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M195" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>218</v>
       </c>
@@ -9017,14 +7832,8 @@
       <c r="K196" t="s">
         <v>17</v>
       </c>
-      <c r="L196" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M196" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>219</v>
       </c>
@@ -9058,14 +7867,8 @@
       <c r="K197" t="s">
         <v>28</v>
       </c>
-      <c r="L197" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M197" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>220</v>
       </c>
@@ -9099,14 +7902,8 @@
       <c r="K198" t="s">
         <v>40</v>
       </c>
-      <c r="L198" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M198" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>221</v>
       </c>
@@ -9126,13 +7923,13 @@
         <v>0</v>
       </c>
       <c r="G199">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J199" t="s">
         <v>16</v>
@@ -9140,14 +7937,8 @@
       <c r="K199" t="s">
         <v>13</v>
       </c>
-      <c r="L199" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="M199" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>222</v>
       </c>
@@ -9177,14 +7968,8 @@
       <c r="K200" t="s">
         <v>13</v>
       </c>
-      <c r="L200" s="1">
-        <v>0</v>
-      </c>
-      <c r="M200" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>223</v>
       </c>
@@ -9218,14 +8003,8 @@
       <c r="K201" t="s">
         <v>37</v>
       </c>
-      <c r="L201" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M201" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>224</v>
       </c>
@@ -9259,14 +8038,8 @@
       <c r="K202" t="s">
         <v>22</v>
       </c>
-      <c r="L202" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M202" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>225</v>
       </c>
@@ -9300,14 +8073,8 @@
       <c r="K203" t="s">
         <v>22</v>
       </c>
-      <c r="L203" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M203" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>226</v>
       </c>
@@ -9341,14 +8108,8 @@
       <c r="K204" t="s">
         <v>22</v>
       </c>
-      <c r="L204" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M204" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>227</v>
       </c>
@@ -9382,14 +8143,8 @@
       <c r="K205" t="s">
         <v>17</v>
       </c>
-      <c r="L205" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M205" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>228</v>
       </c>
@@ -9423,14 +8178,8 @@
       <c r="K206" t="s">
         <v>17</v>
       </c>
-      <c r="L206" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M206" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>229</v>
       </c>
@@ -9464,14 +8213,8 @@
       <c r="K207" t="s">
         <v>17</v>
       </c>
-      <c r="L207" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M207" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>230</v>
       </c>
@@ -9505,14 +8248,8 @@
       <c r="K208" t="s">
         <v>28</v>
       </c>
-      <c r="L208" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M208" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>231</v>
       </c>
@@ -9542,14 +8279,8 @@
       <c r="K209" t="s">
         <v>13</v>
       </c>
-      <c r="L209" s="1">
-        <v>0</v>
-      </c>
-      <c r="M209" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>232</v>
       </c>
@@ -9579,14 +8310,8 @@
       <c r="K210" t="s">
         <v>13</v>
       </c>
-      <c r="L210" s="1">
-        <v>0</v>
-      </c>
-      <c r="M210" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>233</v>
       </c>
@@ -9616,14 +8341,8 @@
       <c r="K211" t="s">
         <v>13</v>
       </c>
-      <c r="L211" s="1">
-        <v>0</v>
-      </c>
-      <c r="M211" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>234</v>
       </c>
@@ -9643,13 +8362,13 @@
         <v>0</v>
       </c>
       <c r="G212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I212">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J212" t="s">
         <v>16</v>
@@ -9657,14 +8376,8 @@
       <c r="K212" t="s">
         <v>13</v>
       </c>
-      <c r="L212" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="M212" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>235</v>
       </c>
@@ -9694,14 +8407,8 @@
       <c r="K213" t="s">
         <v>13</v>
       </c>
-      <c r="L213" s="1">
-        <v>0</v>
-      </c>
-      <c r="M213" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>236</v>
       </c>
@@ -9731,14 +8438,8 @@
       <c r="K214" t="s">
         <v>13</v>
       </c>
-      <c r="L214" s="1">
-        <v>0</v>
-      </c>
-      <c r="M214" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>237</v>
       </c>
@@ -9768,14 +8469,8 @@
       <c r="K215" t="s">
         <v>13</v>
       </c>
-      <c r="L215" s="1">
-        <v>0</v>
-      </c>
-      <c r="M215" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>238</v>
       </c>
@@ -9795,13 +8490,13 @@
         <v>0</v>
       </c>
       <c r="G216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H216">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J216" t="s">
         <v>16</v>
@@ -9809,14 +8504,8 @@
       <c r="K216" t="s">
         <v>13</v>
       </c>
-      <c r="L216" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="M216" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>239</v>
       </c>
@@ -9846,14 +8535,8 @@
       <c r="K217" t="s">
         <v>13</v>
       </c>
-      <c r="L217" s="1">
-        <v>0</v>
-      </c>
-      <c r="M217" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>240</v>
       </c>
@@ -9882,12 +8565,6 @@
       </c>
       <c r="K218" t="s">
         <v>13</v>
-      </c>
-      <c r="L218" s="1">
-        <v>0</v>
-      </c>
-      <c r="M218" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adatfájl változtatás+programok fixálása az első teszt után
</commit_message>
<xml_diff>
--- a/resources/terkep_adatok.xlsx
+++ b/resources/terkep_adatok.xlsx
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="M210" sqref="M210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5140,7 +5140,7 @@
         <v>141</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -5171,7 +5171,7 @@
         <v>142</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -5206,7 +5206,7 @@
         <v>143</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C121">
         <v>3</v>
@@ -5241,7 +5241,7 @@
         <v>144</v>
       </c>
       <c r="B122">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C122">
         <v>4</v>
@@ -5276,7 +5276,7 @@
         <v>145</v>
       </c>
       <c r="B123">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C123">
         <v>5</v>
@@ -5311,7 +5311,7 @@
         <v>146</v>
       </c>
       <c r="B124">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C124">
         <v>6</v>
@@ -5346,7 +5346,7 @@
         <v>147</v>
       </c>
       <c r="B125">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C125">
         <v>7</v>
@@ -5381,7 +5381,7 @@
         <v>148</v>
       </c>
       <c r="B126">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C126">
         <v>8</v>
@@ -5416,7 +5416,7 @@
         <v>149</v>
       </c>
       <c r="B127">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C127">
         <v>9</v>
@@ -5451,7 +5451,7 @@
         <v>150</v>
       </c>
       <c r="B128">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C128">
         <v>10</v>
@@ -5486,7 +5486,7 @@
         <v>151</v>
       </c>
       <c r="B129">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C129">
         <v>11</v>
@@ -5521,7 +5521,7 @@
         <v>152</v>
       </c>
       <c r="B130">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C130">
         <v>12</v>
@@ -5556,7 +5556,7 @@
         <v>153</v>
       </c>
       <c r="B131">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C131">
         <v>13</v>
@@ -5591,7 +5591,7 @@
         <v>154</v>
       </c>
       <c r="B132">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C132">
         <v>14</v>
@@ -5626,7 +5626,7 @@
         <v>155</v>
       </c>
       <c r="B133">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C133">
         <v>15</v>
@@ -5661,7 +5661,7 @@
         <v>156</v>
       </c>
       <c r="B134">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C134">
         <v>16</v>
@@ -5692,7 +5692,7 @@
         <v>157</v>
       </c>
       <c r="B135">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -5727,7 +5727,7 @@
         <v>158</v>
       </c>
       <c r="B136">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C136">
         <v>2</v>
@@ -5762,7 +5762,7 @@
         <v>159</v>
       </c>
       <c r="B137">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -5797,7 +5797,7 @@
         <v>160</v>
       </c>
       <c r="B138">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C138">
         <v>4</v>
@@ -5832,7 +5832,7 @@
         <v>161</v>
       </c>
       <c r="B139">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C139">
         <v>5</v>
@@ -5867,7 +5867,7 @@
         <v>162</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C140">
         <v>6</v>
@@ -5902,7 +5902,7 @@
         <v>163</v>
       </c>
       <c r="B141">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C141">
         <v>7</v>
@@ -5937,7 +5937,7 @@
         <v>164</v>
       </c>
       <c r="B142">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C142">
         <v>8</v>
@@ -5972,7 +5972,7 @@
         <v>165</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C143">
         <v>9</v>
@@ -6007,7 +6007,7 @@
         <v>166</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C144">
         <v>10</v>
@@ -6042,7 +6042,7 @@
         <v>167</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C145">
         <v>11</v>
@@ -6077,7 +6077,7 @@
         <v>168</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C146">
         <v>12</v>
@@ -6112,7 +6112,7 @@
         <v>169</v>
       </c>
       <c r="B147">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C147">
         <v>13</v>
@@ -6147,7 +6147,7 @@
         <v>170</v>
       </c>
       <c r="B148">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C148">
         <v>14</v>
@@ -6182,7 +6182,7 @@
         <v>171</v>
       </c>
       <c r="B149">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C149">
         <v>15</v>
@@ -6217,7 +6217,7 @@
         <v>172</v>
       </c>
       <c r="B150">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -6248,7 +6248,7 @@
         <v>173</v>
       </c>
       <c r="B151">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C151">
         <v>2</v>
@@ -6283,7 +6283,7 @@
         <v>174</v>
       </c>
       <c r="B152">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C152">
         <v>3</v>
@@ -6318,7 +6318,7 @@
         <v>175</v>
       </c>
       <c r="B153">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C153">
         <v>4</v>
@@ -6353,7 +6353,7 @@
         <v>176</v>
       </c>
       <c r="B154">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -6388,7 +6388,7 @@
         <v>177</v>
       </c>
       <c r="B155">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C155">
         <v>6</v>
@@ -6423,7 +6423,7 @@
         <v>178</v>
       </c>
       <c r="B156">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C156">
         <v>7</v>
@@ -6458,7 +6458,7 @@
         <v>179</v>
       </c>
       <c r="B157">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C157">
         <v>8</v>
@@ -6493,7 +6493,7 @@
         <v>180</v>
       </c>
       <c r="B158">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C158">
         <v>9</v>
@@ -6528,7 +6528,7 @@
         <v>181</v>
       </c>
       <c r="B159">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C159">
         <v>10</v>
@@ -6563,7 +6563,7 @@
         <v>182</v>
       </c>
       <c r="B160">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C160">
         <v>11</v>
@@ -6598,7 +6598,7 @@
         <v>183</v>
       </c>
       <c r="B161">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C161">
         <v>12</v>
@@ -6633,7 +6633,7 @@
         <v>184</v>
       </c>
       <c r="B162">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C162">
         <v>13</v>
@@ -6668,7 +6668,7 @@
         <v>185</v>
       </c>
       <c r="B163">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C163">
         <v>14</v>
@@ -6699,7 +6699,7 @@
         <v>186</v>
       </c>
       <c r="B164">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -6730,7 +6730,7 @@
         <v>187</v>
       </c>
       <c r="B165">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C165">
         <v>2</v>
@@ -6765,7 +6765,7 @@
         <v>188</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C166">
         <v>3</v>
@@ -6800,7 +6800,7 @@
         <v>189</v>
       </c>
       <c r="B167">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C167">
         <v>4</v>
@@ -6835,7 +6835,7 @@
         <v>190</v>
       </c>
       <c r="B168">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C168">
         <v>5</v>
@@ -6870,7 +6870,7 @@
         <v>191</v>
       </c>
       <c r="B169">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C169">
         <v>6</v>
@@ -6905,7 +6905,7 @@
         <v>192</v>
       </c>
       <c r="B170">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C170">
         <v>7</v>
@@ -6940,7 +6940,7 @@
         <v>193</v>
       </c>
       <c r="B171">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C171">
         <v>8</v>
@@ -6975,7 +6975,7 @@
         <v>194</v>
       </c>
       <c r="B172">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C172">
         <v>9</v>
@@ -7010,7 +7010,7 @@
         <v>195</v>
       </c>
       <c r="B173">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C173">
         <v>10</v>
@@ -7045,7 +7045,7 @@
         <v>196</v>
       </c>
       <c r="B174">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C174">
         <v>11</v>
@@ -7080,7 +7080,7 @@
         <v>197</v>
       </c>
       <c r="B175">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C175">
         <v>12</v>
@@ -7115,7 +7115,7 @@
         <v>198</v>
       </c>
       <c r="B176">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C176">
         <v>13</v>
@@ -7146,7 +7146,7 @@
         <v>199</v>
       </c>
       <c r="B177">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -7177,7 +7177,7 @@
         <v>200</v>
       </c>
       <c r="B178">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C178">
         <v>2</v>
@@ -7212,7 +7212,7 @@
         <v>201</v>
       </c>
       <c r="B179">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C179">
         <v>3</v>
@@ -7247,7 +7247,7 @@
         <v>202</v>
       </c>
       <c r="B180">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C180">
         <v>4</v>
@@ -7282,7 +7282,7 @@
         <v>203</v>
       </c>
       <c r="B181">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C181">
         <v>5</v>
@@ -7317,7 +7317,7 @@
         <v>204</v>
       </c>
       <c r="B182">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C182">
         <v>6</v>
@@ -7352,7 +7352,7 @@
         <v>205</v>
       </c>
       <c r="B183">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C183">
         <v>7</v>
@@ -7387,7 +7387,7 @@
         <v>206</v>
       </c>
       <c r="B184">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C184">
         <v>8</v>
@@ -7422,7 +7422,7 @@
         <v>207</v>
       </c>
       <c r="B185">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C185">
         <v>9</v>
@@ -7457,7 +7457,7 @@
         <v>208</v>
       </c>
       <c r="B186">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C186">
         <v>10</v>
@@ -7492,7 +7492,7 @@
         <v>209</v>
       </c>
       <c r="B187">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C187">
         <v>11</v>
@@ -7527,7 +7527,7 @@
         <v>210</v>
       </c>
       <c r="B188">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C188">
         <v>12</v>
@@ -7558,7 +7558,7 @@
         <v>211</v>
       </c>
       <c r="B189">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -7593,7 +7593,7 @@
         <v>212</v>
       </c>
       <c r="B190">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C190">
         <v>2</v>
@@ -7628,7 +7628,7 @@
         <v>213</v>
       </c>
       <c r="B191">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -7663,7 +7663,7 @@
         <v>214</v>
       </c>
       <c r="B192">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C192">
         <v>4</v>
@@ -7698,7 +7698,7 @@
         <v>215</v>
       </c>
       <c r="B193">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C193">
         <v>5</v>
@@ -7733,7 +7733,7 @@
         <v>216</v>
       </c>
       <c r="B194">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C194">
         <v>6</v>
@@ -7768,7 +7768,7 @@
         <v>217</v>
       </c>
       <c r="B195">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C195">
         <v>7</v>
@@ -7803,7 +7803,7 @@
         <v>218</v>
       </c>
       <c r="B196">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C196">
         <v>8</v>
@@ -7838,7 +7838,7 @@
         <v>219</v>
       </c>
       <c r="B197">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C197">
         <v>9</v>
@@ -7873,7 +7873,7 @@
         <v>220</v>
       </c>
       <c r="B198">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C198">
         <v>10</v>
@@ -7908,7 +7908,7 @@
         <v>221</v>
       </c>
       <c r="B199">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C199">
         <v>11</v>
@@ -7943,7 +7943,7 @@
         <v>222</v>
       </c>
       <c r="B200">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -7974,7 +7974,7 @@
         <v>223</v>
       </c>
       <c r="B201">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C201">
         <v>2</v>
@@ -8009,7 +8009,7 @@
         <v>224</v>
       </c>
       <c r="B202">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C202">
         <v>3</v>
@@ -8044,7 +8044,7 @@
         <v>225</v>
       </c>
       <c r="B203">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C203">
         <v>4</v>
@@ -8079,7 +8079,7 @@
         <v>226</v>
       </c>
       <c r="B204">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C204">
         <v>5</v>
@@ -8114,7 +8114,7 @@
         <v>227</v>
       </c>
       <c r="B205">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C205">
         <v>6</v>
@@ -8149,7 +8149,7 @@
         <v>228</v>
       </c>
       <c r="B206">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C206">
         <v>7</v>
@@ -8184,7 +8184,7 @@
         <v>229</v>
       </c>
       <c r="B207">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C207">
         <v>8</v>
@@ -8219,7 +8219,7 @@
         <v>230</v>
       </c>
       <c r="B208">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C208">
         <v>9</v>
@@ -8254,7 +8254,7 @@
         <v>231</v>
       </c>
       <c r="B209">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C209">
         <v>10</v>
@@ -8285,7 +8285,7 @@
         <v>232</v>
       </c>
       <c r="B210">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -8316,7 +8316,7 @@
         <v>233</v>
       </c>
       <c r="B211">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C211">
         <v>2</v>
@@ -8347,7 +8347,7 @@
         <v>234</v>
       </c>
       <c r="B212">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C212">
         <v>3</v>
@@ -8382,7 +8382,7 @@
         <v>235</v>
       </c>
       <c r="B213">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C213">
         <v>4</v>
@@ -8413,7 +8413,7 @@
         <v>236</v>
       </c>
       <c r="B214">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C214">
         <v>5</v>
@@ -8444,7 +8444,7 @@
         <v>237</v>
       </c>
       <c r="B215">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C215">
         <v>6</v>
@@ -8475,7 +8475,7 @@
         <v>238</v>
       </c>
       <c r="B216">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C216">
         <v>7</v>
@@ -8510,7 +8510,7 @@
         <v>239</v>
       </c>
       <c r="B217">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C217">
         <v>8</v>
@@ -8541,7 +8541,7 @@
         <v>240</v>
       </c>
       <c r="B218">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C218">
         <v>9</v>

</xml_diff>